<commit_message>
Update to miRetrieve 1.3.2
Added conversion of non-ASCII to ASCII
Added miRetrieve website
</commit_message>
<xml_diff>
--- a/data-raw/stopwords.xlsx
+++ b/data-raw/stopwords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julian/Documents/Jupyter/miRetrieve pkg/miRetrieve/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julian/Documents/Jupyter/miRetrieve/miRetrieve/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D7C302-756C-D140-8353-A0287B3EEBFF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0E0907-5697-DC41-A343-11D01FF96A5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8468" uniqueCount="8457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8471" uniqueCount="8460">
   <si>
     <t>word</t>
   </si>
@@ -25391,6 +25391,15 @@
   </si>
   <si>
     <t>cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">α </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> α </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> α</t>
   </si>
 </sst>
 </file>
@@ -25724,10 +25733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A8468"/>
+  <dimension ref="A1:A8471"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A8451" workbookViewId="0">
+      <selection activeCell="A8464" sqref="A8464"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -68072,6 +68081,21 @@
         <v>8455</v>
       </c>
     </row>
+    <row r="8469" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8469" t="s">
+        <v>8457</v>
+      </c>
+    </row>
+    <row r="8470" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8470" t="s">
+        <v>8458</v>
+      </c>
+    </row>
+    <row r="8471" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8471" t="s">
+        <v>8459</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>